<commit_message>
modification images contrastes et structures , le formulaire dt etre amélioré + h4
</commit_message>
<xml_diff>
--- a/cour/Modèle-audit-SEO (1).xlsx
+++ b/cour/Modèle-audit-SEO (1).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="115">
   <si>
     <t>Catégorie</t>
   </si>
@@ -42,21 +42,12 @@
     <t>(SEO ou accessiblité ?)</t>
   </si>
   <si>
-    <t xml:space="preserve">les images sont trop lourdes             </t>
-  </si>
-  <si>
-    <t>trop lourdes , telechargement trop long</t>
-  </si>
-  <si>
     <t>téléchargement non optimisé</t>
   </si>
   <si>
     <t>verifier que la compression ai bien été activée</t>
   </si>
   <si>
-    <t>le contenue ne sadapte mal aux différents ecrans</t>
-  </si>
-  <si>
     <t>tout site doit être respondive avec version mobile ++</t>
   </si>
   <si>
@@ -72,12 +63,6 @@
     <t xml:space="preserve">accessibilité   </t>
   </si>
   <si>
-    <t>accessibilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">non perceptible , contraste visuel non suffisant </t>
-  </si>
-  <si>
     <t>on page/ SEO</t>
   </si>
   <si>
@@ -87,111 +72,48 @@
     <t>on page /  SEO</t>
   </si>
   <si>
-    <t>img idem contenant</t>
-  </si>
-  <si>
-    <t>liens partenaires en bas de page</t>
-  </si>
-  <si>
     <t>les liens permettent d'augmenté lautorité et dc accessibilité, doivent etre de qualité et haut de page</t>
   </si>
   <si>
-    <t>police des paragraphes trop petites</t>
-  </si>
-  <si>
     <t>travailler sur les mots clés, mettre en valeur lentreprise avec description photo adresse etc au niveau page contact</t>
   </si>
   <si>
     <t>code visibilité pas bon</t>
   </si>
   <si>
-    <t xml:space="preserve">il faut utliser hidden , visibility </t>
-  </si>
-  <si>
     <t xml:space="preserve">l faut utliser hidden , visibility et jamais z index  </t>
   </si>
   <si>
     <t xml:space="preserve"> z-index: 100000 pour visiblité</t>
   </si>
   <si>
-    <t xml:space="preserve">le texte doit etre en dehors de limage </t>
-  </si>
-  <si>
-    <t>mettre le texte a coté de l'image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le texte est dans limage </t>
-  </si>
-  <si>
     <t xml:space="preserve"> texte dans image= probleme de vivibilité et ne peut etre grossit </t>
   </si>
   <si>
     <t xml:space="preserve"> liens ac reseaux sociaux / liens partenaires en haut de page( au lieu de répéter un logo mettre les liens et le beau logo en haut)</t>
   </si>
   <si>
-    <t>h1 puis h3 puis h2 puis h4  , pas de mot clés dans les titres  et manque dans paragraphe</t>
-  </si>
-  <si>
     <t xml:space="preserve"> liens en page accueil en ht++, partenariat , reseaux</t>
   </si>
   <si>
-    <t xml:space="preserve"> h1  avec mots clés h2 mot clé ou synonimes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">langue de la page mal définie </t>
-  </si>
-  <si>
     <t>la langue est elle définie par programmation?</t>
   </si>
   <si>
     <t xml:space="preserve">définir correctement la langue de la page </t>
   </si>
   <si>
-    <t>formulaire de saisie page 2</t>
-  </si>
-  <si>
-    <t>pas d'indication  à l'entrée des informations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">les erreures doivent etre clairement décrites, il doit y avoir des instructions </t>
-  </si>
-  <si>
-    <t>mauvais contraste texte dans image, bloc3 et bloc 1 et bloc footer</t>
-  </si>
-  <si>
     <t xml:space="preserve">les bloc de textes ne sont pas alignés correctement </t>
   </si>
   <si>
     <t xml:space="preserve">il faut que le contenue soit liible perceptible comprehensible </t>
   </si>
   <si>
-    <t>WCA G2 w3c working group note</t>
-  </si>
-  <si>
     <t>contenu mal organisé: ordre des titres et leur mots clés, contenu vide li</t>
   </si>
   <si>
-    <t>WCA G2 w3c working group note AA</t>
-  </si>
-  <si>
-    <t>WCA G2 w3c working group note A</t>
-  </si>
-  <si>
     <t xml:space="preserve">,description vide,page non decrite commme etant l'originale. pas dindex follow, pause pb doptimisation  et de référencement </t>
   </si>
   <si>
-    <t>balise metas manquantes: title description canonical lang robot + manque mot clés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equivalent textuel " alt" qui décrit succintement limage mais avec mot clé pour referencement  5 à 6 mots précis </t>
-  </si>
-  <si>
-    <t>les mots clés doivent apparaitre,  les metas qui facilitent le SEO doivent apparaitrent soit title description content type robot canonical lang(contentu compréhensible)</t>
-  </si>
-  <si>
-    <t>contenu utilisable:h1 h2 bien structuré du plus spé au plus général, avec des mot clés , mots clés ou synonyme pour h2 ,au moins 1 dans chaque para</t>
-  </si>
-  <si>
     <t>décalé sur la droite nest pas lisible /accessible/ pas cohérent par rapport a page d'accueil/ toggle nav nexiste pas sur la page d'accueil</t>
   </si>
   <si>
@@ -216,42 +138,516 @@
     <t>accessibilité  choisi</t>
   </si>
   <si>
-    <t xml:space="preserve"> regles WCAG contraste doit etre de 3,1(pour texte de grande taille).  le contraste entre le texte et larr plan de 4,5:1
+    <t>openclassroom.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ne facilitent pas le téléchargement car fichiers trop lourd cc et js , </t>
+  </si>
+  <si>
+    <t>stockage données dans un cache , zone temporaire gagne tempspour le chargeent de la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vitesse SEO  </t>
+  </si>
+  <si>
+    <t>responsive pas adapté, google utilise la version mobile pour le classement et l'indexation</t>
+  </si>
+  <si>
+    <t>pas une bonne lisibilité , la typo n'est pas accesible car aperture fermée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regles WCAG aperture ouverte trait uniforme </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=créer une design visuel accessible avec la typographie.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> aperture ouverte</t>
+    </r>
+  </si>
+  <si>
+    <t>SEO on page choisi</t>
+  </si>
+  <si>
+    <t>les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=rendre limage compréhensible et améliorer le positionnement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> corriger le alt + court avec mot clé</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">objectif=augmentter le référencement la classification et le renseignement </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">il faut rajouter cela dans le head </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=rendre le formulaire compréhensible</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> .rajouter un code couleur notification pour guider l'utilisateur</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif: facilité la navigation des utilisateur des tech d'assistance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> modifier la structure: header   main   footer</t>
+    </r>
+  </si>
+  <si>
+    <t>mauvaise structure hierarchique, que des div , les blocs ne sont pas clairement délimités</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pas d'architecture cohérante, la page nest pas bien cartographier la navigation pas facilité</t>
+  </si>
+  <si>
+    <t>contenu doit etre bien segmenté,contenu optimisé avec des elements html structurels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilité  </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">objectif=rendre le code lisible </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ajouter dans le head lang em ou fr</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO on page </t>
+  </si>
+  <si>
+    <t>contenu utilisable:h1 h2 bien structuré du plus spé au plus général, avec des mot clés , mots clés ou synonyme pour h2 ,au moins 1 dans chaque paragraphe</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif= alleger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.reduction taille manuelle </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>découper limage + compression avec imageoptim+ reSmush.it</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> optimisation,lossy :perte qualité mais + léger</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif= optimiser le téléchargement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> .parametrer en tete http  dans </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>fichier htaccess</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">, utiliser </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>cache cheaker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> pour tester</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> objectif=rendre le contenu utilisable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> h1  avec mots clés h2 mot clé ou synonimes, vérifier la structure avec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> webaim wave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=alléger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>GZIP pour la compression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">(reduit le nbr de demande et reponde http jusqu'à 70%) des fichiers  se fassent auto  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>minification  js css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>(diminu le poid du fichier)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>www.minifier.org</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> regles WCAG contraste doit etre de 3,1(pour texte de grande taille).  le contraste entre le texte et larr plan de 4,5:1 pour texte normaux
 regles WCAG contreforme ouverte trait uniforme interlettrage et interligne </t>
   </si>
   <si>
-    <t>fichiers trop lourds , css et js 14% du poid total de la page web</t>
-  </si>
-  <si>
-    <t>kinsta.com openclassroom.com</t>
-  </si>
-  <si>
-    <t>openclassroom.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ne facilitent pas le téléchargement car fichiers trop lourd cc et js , </t>
-  </si>
-  <si>
-    <t>pas de cache navigateur:zone de stockage temporaire et rapide</t>
-  </si>
-  <si>
+    <t>il faut utliser hidden , visibility mais jamais utiliser lopacité nulle l'ordre des z index pour le masquage de contenu .l'élément doit être réelement invisible.</t>
+  </si>
+  <si>
+    <t>le texte doit etre en dehors de limage , les images avec du texte doivent être évités</t>
+  </si>
+  <si>
+    <t>pas de cache navigateur:zone de stockage temporaire et rapide ( pas installable avec git hub)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">les images sont trop lourdes : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">img 1 et 2 ;img citation;banniere , la chouette agence ,logo         </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=alléger</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>. GZIP pour la compression(reduit le nbr de demande et reponde http jusqu'à 70%) des fichiers  se fassent auto  minification  js css(diminu le poid du fichier)</t>
+        <color rgb="FF7030A0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mauvais contraste texte dans image, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bloc3 et bloc 1 et bloc footer,au niveau du logo la chouette A,du bouton contact</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">liens vident au niveaux des réseaux sociaux et liens redondants entre accueil et contact et contactez notre équipe </t>
+  </si>
+  <si>
+    <t>soit on en enlève les liens soit on apporte du texte pour décrire leur fonctionalité ,</t>
+  </si>
+  <si>
+    <t>equivalent textuel " alt" qui décrit succintement limage mais avec mot clé pour referencement  5 à 6 mots précis , il ne faut pas répéter le même alt</t>
+  </si>
+  <si>
+    <t>h1 puis h3 puis h2   , pas de mot clés dans les titres  et manque dans paragraphe</t>
+  </si>
+  <si>
+    <t>non perceptible , contraste visuel non suffisant pour les personnes à capacité visuelle réduite</t>
+  </si>
+  <si>
+    <t>trop lourdes , telechargement trop long: la taille est modifié via le css</t>
+  </si>
+  <si>
+    <t>les liens vers reseauux sociaux sont vident  ne sont pas compréhensibles pour l'utilisateur et n'apporte rien au site . Redondances sur la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WCA G2 w3c working group note AA , wave web evaluation tool, </t>
+  </si>
+  <si>
+    <t>WCA G2 w3c working group note AA , wave web evaluation tool, mdn web doc ,  https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-contrast.html</t>
+  </si>
+  <si>
+    <t>WCA G2 w3c working group note AA                                                                 https://www.w3.org/TR/UNDERSTANDING-WCAG20/consistent-behavior-consistent-locations.html</t>
+  </si>
+  <si>
+    <t>police des paragraphes trop petites ,la chouette agence police trop petite</t>
+  </si>
+  <si>
+    <r>
+      <t>WCA G2 w3c working group note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A                                                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-parses.html</t>
+    </r>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941044-inspectez-manuellement-le-contenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/UNDERSTANDING-WCAG20/content-structure-separation-programmatic.html     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941044-inspectez-manuellement-le-contenu </t>
+  </si>
+  <si>
+    <r>
+      <t>WCA G2 w3c working group note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A                         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    https://www.balisemeta.com/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>WCA G2 w3c working group note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                  wave web evaluation tool   , https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-parses.html      https://validator.w3.org/nu/?doc=https%3A%2F%2Flazouz44.github.io%2Fla-chouette-agence%2F</t>
     </r>
   </si>
   <si>
@@ -263,19 +659,17 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>objectif= alleger</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.reduction taille manuelle découper limage + compression avec imageoptim+ reSmush.it optimisation,lossy :perte qualité mais + léger</t>
-    </r>
-  </si>
-  <si>
+      <t>objectif=créer une design visuel accessible avec les contrastes de couleur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.augmenter le contraste entre le texte et background</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -284,31 +678,44 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>objectif= optimiser le téléchargement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> .parametrer en tete http  dans fichier htaccess, utiliser cache cheaker pour tester</t>
-    </r>
-  </si>
-  <si>
-    <t>stockage données dans un cache , zone temporaire gagne tempspour le chargeent de la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vitesse SEO  </t>
-  </si>
-  <si>
-    <t>responsive pas adapté, google utilise la version mobile pour le classement et l'indexation</t>
-  </si>
-  <si>
-    <t>pas une bonne lisibilité , la typo n'est pas accesible car aperture fermée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regles WCAG aperture ouverte trait uniforme </t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">test avec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>contrast analizer  web-color.alias</t>
+    </r>
+  </si>
+  <si>
+    <t>le alt  ne décrit pas bien  chaque image(paris au lieu de lyon par ex)/ redondance au niveau de 2 alt avec même description</t>
+  </si>
+  <si>
+    <t>les erreures doivent etre clairement décrites, il doit y avoir des instructions , réécrire le code formulaire</t>
+  </si>
+  <si>
+    <t>pas d'indication  à l'entrée des informations , pas etiquette: pause pb pour le lecteur d'écran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image doit avoir l même taille que son contenant </t>
+  </si>
+  <si>
+    <t>les mots clés doivent apparaitre,  les metas qui facilitent le SEO doivent apparaitrent soit title description content type robot canonical (contentu compréhensible)</t>
+  </si>
+  <si>
+    <t>le contenue ne sadapte mal au mobile : des images ne sont pas lisibles .</t>
   </si>
   <si>
     <r>
@@ -319,251 +726,167 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>objectif=créer une design visuel accessible avec la typographie.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> aperture ouverte</t>
-    </r>
-  </si>
-  <si>
+      <t>objectif=augmenter le trafic avec un site responsive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> .créer une super version mobile avec images titres bien visibles </t>
+    </r>
+  </si>
+  <si>
+    <t>liens partenaires en bas de page ++ balxk hat a supprimé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">du texte invisible est créé en haut à gauche pour stocker des mots clés cest du black hat trompe google ,  très mauvaise pratique </t>
+  </si>
+  <si>
+    <t>SEO on page  choisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilité </t>
+  </si>
+  <si>
+    <t>de faux liens sont utllisé au niveau de l'annuaire et partenariat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut les enlever et au mieux rajouter de vrais liens externes et vrais partenariariat qui apportent quelque chose au site </t>
+  </si>
+  <si>
+    <t>objectif=être partagé sur les réseaux sociaux, augmenter l'autorité du site    , renseigner les liens , retirer les liens redondant (garder contact)</t>
+  </si>
+  <si>
+    <t>objectif=rendre le menu lisible il faut deplacer le menu pour quil soit visible</t>
+  </si>
+  <si>
+    <t>objectif= rendre le contenu utilisable et avec de bonnes pratiques</t>
+  </si>
+  <si>
+    <t>accessibilité choisi</t>
+  </si>
+  <si>
+    <t>objectif=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdn web doc  https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-text-presentation.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WCA G2 w3c working group note / Optimiz me  /   wave web evaluation tool  ,  https://www.w3.org/TR/UNDERSTANDING-WCAG20/text-equiv-all.html  working group note AA  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pratique black hat : de faux liens sont utilisés au niveau du footer </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=créer une design visuel accessible avec les contrastes de couleur.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>changé la couleur du texte rouge , enlevé le texte de limage pour les 2 blocs</t>
-    </r>
-  </si>
-  <si>
-    <t>SEO on page choisi</t>
-  </si>
-  <si>
-    <t>les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
-  </si>
-  <si>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  oke</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">le texte est dans limage , la citation  et le titre </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=rendre limage compréhensible et améliorer le positionnement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> corriger le alt + court avec mot clé</t>
-    </r>
-  </si>
-  <si>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> oke</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">langue de la page mal définie    </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">objectif=augmentter le référencement la classification et le renseignement </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">il faut rajouter cela dans le head </t>
-    </r>
-  </si>
-  <si>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>oke</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">creation de div keyords non  autorisées texte trop petit     black hat   </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=augmenter le trafic avec un site responsive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> .créer une super version mobile</t>
-    </r>
-  </si>
-  <si>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>oke</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">balise metas manquantes: title description canonical  robot + manque mot clés  </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=rendre le formulaire compréhensible</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> .rajouter un code couleur notification pour guider l'utilisateur</t>
-    </r>
-  </si>
-  <si>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">oke </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>formulaire de saisie page 2</t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FF00B050"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>objectif=rendre le menu lisible</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
+      <t xml:space="preserve"> zone de texte a rajouter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>fichiers trop lourds , css et js 14% du poid total de la page web (source httparchive)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> il faut deplacer e menu pour quil soit visible</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif: facilité la navigation des utilisateur des tech d'assistance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> modifier la structure: header   main   footer</t>
-    </r>
-  </si>
-  <si>
-    <t>accessibilité  ou</t>
-  </si>
-  <si>
-    <t>mauvaise structure hierarchique, que des div , les blocs ne sont pas clairement délimités</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pas d'architecture cohérante, la page nest pas bien cartographier la navigation pas facilité</t>
-  </si>
-  <si>
-    <t>contenu doit etre bien segmenté,contenu optimisé avec des elements html structurels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choisir entre formulaire menu et struture  manque 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">accessibilité  </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">objectif=rendre le code lisible </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ajouter dans le head lang em ou fr</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">balise id non unique </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEO on page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">les liens sont vident  ne sont pas compréhensibles pour l'utilisateur et n'apporte rien au site . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">soit on en enlève les liens soit on apporte du texte pour décrire leur fonctionalité </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">objectif=être partagé sur les réseaux sociaux, augmenter l'autorité du site    , </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">renseigner les liens </t>
-    </r>
-  </si>
-  <si>
-    <t>WCA G2 w3c working group note AA , wave web evaluation tool</t>
-  </si>
-  <si>
-    <t>WCA G2 w3c working group note / Optimiz me   wave web evaluation tool</t>
-  </si>
-  <si>
-    <t>WCA G2 w3c working group note A                       wave web evaluation tool</t>
-  </si>
-  <si>
-    <t>le alt est surchargée et ne décrit pas bien  chaque image répétition, il faut un mot clé :pb pour personne mal voyante , si img ne saffiche pas</t>
-  </si>
-  <si>
-    <t>liens vident au niveaux des réseaux sociaux et liens redondants</t>
+      <t xml:space="preserve"> ala fin</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -612,14 +935,39 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF7030A0"/>
+      <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -654,10 +1002,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -665,17 +1014,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -888,18 +1237,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="122.5546875" customWidth="1"/>
-    <col min="3" max="3" width="114.88671875" customWidth="1"/>
-    <col min="4" max="4" width="133.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="138" customWidth="1"/>
     <col min="5" max="5" width="139" customWidth="1"/>
-    <col min="6" max="6" width="71.33203125" customWidth="1"/>
+    <col min="6" max="6" width="212.77734375" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -953,367 +1302,399 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
+        <v>91</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
+        <v>59</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>66</v>
+        <v>35</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" t="s">
-        <v>68</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
+      <c r="A8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>68</v>
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>53</v>
+        <v>35</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>84</v>
+        <v>92</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>76</v>
+        <v>36</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>101</v>
+        <v>37</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>68</v>
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>68</v>
+      <c r="A15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>32</v>
+      <c r="A16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>102</v>
+      <c r="A17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>39</v>
+      <c r="A18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>103</v>
+        <v>26</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>42</v>
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="F19" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>58</v>
+        <v>98</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" t="s">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
-        <v>93</v>
-      </c>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2290,7 +2671,15 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="F10" r:id="rId5"/>
+    <hyperlink ref="F21" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
js et css minifiés , manque style .css
</commit_message>
<xml_diff>
--- a/cour/Modèle-audit-SEO (1).xlsx
+++ b/cour/Modèle-audit-SEO (1).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
   <si>
     <t>Catégorie</t>
   </si>
@@ -45,36 +45,15 @@
     <t>téléchargement non optimisé</t>
   </si>
   <si>
-    <t>verifier que la compression ai bien été activée</t>
-  </si>
-  <si>
-    <t>tout site doit être respondive avec version mobile ++</t>
-  </si>
-  <si>
     <t>site pas mis en valeur</t>
   </si>
   <si>
-    <t>mot clé web design dans url, courte ou longue traine?localisation mot clé, analyse google analitics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pas de travail sur mots clés ,  pas de présentation entreprise, </t>
-  </si>
-  <si>
     <t xml:space="preserve">accessibilité   </t>
   </si>
   <si>
     <t>on page/ SEO</t>
   </si>
   <si>
-    <t>on page/   SEO</t>
-  </si>
-  <si>
-    <t>on page /  SEO</t>
-  </si>
-  <si>
-    <t>les liens permettent d'augmenté lautorité et dc accessibilité, doivent etre de qualité et haut de page</t>
-  </si>
-  <si>
     <t>travailler sur les mots clés, mettre en valeur lentreprise avec description photo adresse etc au niveau page contact</t>
   </si>
   <si>
@@ -93,24 +72,9 @@
     <t xml:space="preserve"> liens ac reseaux sociaux / liens partenaires en haut de page( au lieu de répéter un logo mettre les liens et le beau logo en haut)</t>
   </si>
   <si>
-    <t xml:space="preserve"> liens en page accueil en ht++, partenariat , reseaux</t>
-  </si>
-  <si>
     <t>la langue est elle définie par programmation?</t>
   </si>
   <si>
-    <t xml:space="preserve">définir correctement la langue de la page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">les bloc de textes ne sont pas alignés correctement </t>
-  </si>
-  <si>
-    <t xml:space="preserve">il faut que le contenue soit liible perceptible comprehensible </t>
-  </si>
-  <si>
-    <t>contenu mal organisé: ordre des titres et leur mots clés, contenu vide li</t>
-  </si>
-  <si>
     <t xml:space="preserve">,description vide,page non decrite commme etant l'originale. pas dindex follow, pause pb doptimisation  et de référencement </t>
   </si>
   <si>
@@ -129,36 +93,21 @@
     <t>vitesse SEO  choisi</t>
   </si>
   <si>
-    <t>on page/SEO  choisi</t>
-  </si>
-  <si>
-    <t>accessibilité   choisi</t>
-  </si>
-  <si>
-    <t>accessibilité  choisi</t>
-  </si>
-  <si>
     <t>openclassroom.com</t>
   </si>
   <si>
-    <t xml:space="preserve">ne facilitent pas le téléchargement car fichiers trop lourd cc et js , </t>
-  </si>
-  <si>
-    <t>stockage données dans un cache , zone temporaire gagne tempspour le chargeent de la page</t>
-  </si>
-  <si>
     <t xml:space="preserve">vitesse SEO  </t>
   </si>
   <si>
-    <t>responsive pas adapté, google utilise la version mobile pour le classement et l'indexation</t>
-  </si>
-  <si>
     <t>pas une bonne lisibilité , la typo n'est pas accesible car aperture fermée</t>
   </si>
   <si>
     <t xml:space="preserve">regles WCAG aperture ouverte trait uniforme </t>
   </si>
   <si>
+    <t>les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -167,7 +116,398 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>objectif=créer une design visuel accessible avec la typographie.</t>
+      <t xml:space="preserve">objectif=augmentter le référencement la classification et le renseignement </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">il faut rajouter cela dans le head </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif: facilité la navigation des utilisateur des tech d'assistance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> modifier la structure: header   main   footer</t>
+    </r>
+  </si>
+  <si>
+    <t>mauvaise structure hierarchique, que des div , les blocs ne sont pas clairement délimités</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pas d'architecture cohérante, la page nest pas bien cartographier la navigation pas facilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilité  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO on page </t>
+  </si>
+  <si>
+    <t>pas de cache navigateur:zone de stockage temporaire et rapide ( pas installable avec git hub)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liens vident au niveaux des réseaux sociaux et liens redondants entre accueil et contact et contactez notre équipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WCA G2 w3c working group note AA , wave web evaluation tool, </t>
+  </si>
+  <si>
+    <t>WCA G2 w3c working group note AA , wave web evaluation tool, mdn web doc ,  https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-contrast.html</t>
+  </si>
+  <si>
+    <t>WCA G2 w3c working group note AA                                                                 https://www.w3.org/TR/UNDERSTANDING-WCAG20/consistent-behavior-consistent-locations.html</t>
+  </si>
+  <si>
+    <t>police des paragraphes trop petites ,la chouette agence police trop petite</t>
+  </si>
+  <si>
+    <r>
+      <t>WCA G2 w3c working group note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A                                                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-parses.html</t>
+    </r>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941044-inspectez-manuellement-le-contenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/UNDERSTANDING-WCAG20/content-structure-separation-programmatic.html     </t>
+  </si>
+  <si>
+    <r>
+      <t>WCA G2 w3c working group note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A                         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    https://www.balisemeta.com/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>WCA G2 w3c working group note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                  wave web evaluation tool   , https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-parses.html      https://validator.w3.org/nu/?doc=https%3A%2F%2Flazouz44.github.io%2Fla-chouette-agence%2F</t>
+    </r>
+  </si>
+  <si>
+    <t>le alt  ne décrit pas bien  chaque image(paris au lieu de lyon par ex)/ redondance au niveau de 2 alt avec même description</t>
+  </si>
+  <si>
+    <t>pas d'indication  à l'entrée des informations , pas etiquette: pause pb pour le lecteur d'écran</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=augmenter le trafic avec un site responsive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> .créer une super version mobile avec images titres bien visibles </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilité </t>
+  </si>
+  <si>
+    <t>objectif=être partagé sur les réseaux sociaux, augmenter l'autorité du site    , renseigner les liens , retirer les liens redondant (garder contact)</t>
+  </si>
+  <si>
+    <t>objectif=rendre le menu lisible il faut deplacer le menu pour quil soit visible</t>
+  </si>
+  <si>
+    <t>objectif=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdn web doc  https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-text-presentation.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WCA G2 w3c working group note / Optimiz me  /   wave web evaluation tool  ,  https://www.w3.org/TR/UNDERSTANDING-WCAG20/text-equiv-all.html  working group note AA  </t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liens partenaires en bas de page </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> objectif=rendre le CONTENU UTILISABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> h1  avec mots clés h2 mot clé ou synonimes, vérifier la structure avec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> webaim wave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=ALLEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>GZIP pour la compression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">(reduit le nbr de demande et reponde http jusqu'à 70%) des fichiers  se fassent auto  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>minification  js css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>(diminu le poid du fichier)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>www.minifier.org</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif= OPTIMISER le téléchargement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> .parametrer en tete http  dans </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>fichier htaccess</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">, utiliser </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>cache cheaker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> pour tester</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=créer une design visuel ACCESSIBLE avec les contrastes de couleur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.augmenter le contraste entre le texte et background</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">test avec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>contrast analizer  web-color.alias</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=créer une design visuel ACCESSIBLE avec la typographie.</t>
     </r>
     <r>
       <rPr>
@@ -179,12 +519,6 @@
     </r>
   </si>
   <si>
-    <t>SEO on page choisi</t>
-  </si>
-  <si>
-    <t>les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -193,7 +527,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>objectif=rendre limage compréhensible et améliorer le positionnement</t>
+      <t>objectif=rendre limage COMPREHENSIBLE et améliorer le positionnement</t>
     </r>
     <r>
       <rPr>
@@ -213,16 +547,15 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">objectif=augmentter le référencement la classification et le renseignement </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">il faut rajouter cela dans le head </t>
+      <t xml:space="preserve">objectif=rendre le code LISIBLE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ajouter dans le head lang em ou fr</t>
     </r>
   </si>
   <si>
@@ -234,7 +567,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>objectif=rendre le formulaire compréhensible</t>
+      <t>objectif=rendre le formulaire COMPREHENSIBLE</t>
     </r>
     <r>
       <rPr>
@@ -247,639 +580,267 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">pratique black hat : de faux liens sont utilisés au niveau du footer </t>
+    </r>
+    <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif: facilité la navigation des utilisateur des tech d'assistance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> modifier la structure: header   main   footer</t>
-    </r>
-  </si>
-  <si>
-    <t>mauvaise structure hierarchique, que des div , les blocs ne sont pas clairement délimités</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pas d'architecture cohérante, la page nest pas bien cartographier la navigation pas facilité</t>
-  </si>
-  <si>
-    <t>contenu doit etre bien segmenté,contenu optimisé avec des elements html structurels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accessibilité  </t>
-  </si>
-  <si>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">objectif=rendre le code lisible </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ajouter dans le head lang em ou fr</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SEO on page </t>
-  </si>
-  <si>
-    <t>contenu utilisable:h1 h2 bien structuré du plus spé au plus général, avec des mot clés , mots clés ou synonyme pour h2 ,au moins 1 dans chaque paragraphe</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif= alleger</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.reduction taille manuelle </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>découper limage + compression avec imageoptim+ reSmush.it</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> optimisation,lossy :perte qualité mais + léger</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif= optimiser le téléchargement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> .parametrer en tete http  dans </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>fichier htaccess</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">, utiliser </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>cache cheaker</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> pour tester</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> objectif=rendre le contenu utilisable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> h1  avec mots clés h2 mot clé ou synonimes, vérifier la structure avec</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> webaim wave</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=alléger</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>GZIP pour la compression</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">(reduit le nbr de demande et reponde http jusqu'à 70%) des fichiers  se fassent auto  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>minification  js css</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>(diminu le poid du fichier)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>www.minifier.org</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> regles WCAG contraste doit etre de 3,1(pour texte de grande taille).  le contraste entre le texte et larr plan de 4,5:1 pour texte normaux
-regles WCAG contreforme ouverte trait uniforme interlettrage et interligne </t>
-  </si>
-  <si>
-    <t>il faut utliser hidden , visibility mais jamais utiliser lopacité nulle l'ordre des z index pour le masquage de contenu .l'élément doit être réelement invisible.</t>
-  </si>
-  <si>
-    <t>le texte doit etre en dehors de limage , les images avec du texte doivent être évités</t>
-  </si>
-  <si>
-    <t>pas de cache navigateur:zone de stockage temporaire et rapide ( pas installable avec git hub)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">les images sont trop lourdes : </t>
-    </r>
-    <r>
-      <rPr>
         <sz val="12"/>
         <color rgb="FF7030A0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">img 1 et 2 ;img citation;banniere , la chouette agence ,logo         </t>
-    </r>
+      <t xml:space="preserve">et creation de div keyords non  autorisées texte trop petit      </t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> rendre le contenu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>UTILISABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et avec de bonnes pratiques</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>accessibilité          choisi</t>
+  </si>
+  <si>
+    <t>SEO on page       choisi</t>
+  </si>
+  <si>
+    <t>on page/SEO        choisi</t>
+  </si>
+  <si>
+    <t>vitesse SEO          choisi</t>
+  </si>
+  <si>
+    <t>h1 puis h3 puis h2   , pas de mots clés dans les titres  et manque dans paragraphe.</t>
+  </si>
+  <si>
+    <t>Les liens permettent d'augmenter l'autorité et donc l'accessibilité, doivent être de qualité et au mieux en  haut de page.</t>
+  </si>
+  <si>
+    <t>Trop lourdes , téléchargement trop long: la taille est modifiée via le css , le format nest pas optimum .</t>
+  </si>
+  <si>
+    <t>Ne facilitent pas le téléchargement car les fichiers sont  trop lourds : css js , html</t>
+  </si>
+  <si>
+    <t>L'image doit avoir la même taille que son contenant ou plus petite.Il faut privilégier les formats jpg, png voir jpeg 2000 .</t>
+  </si>
+  <si>
+    <t>Le contenu doit être utilisable: h1 h2 bien structuré du plus spécifique au plus général, avec des mot clés , mots clés ou synonyme pour h2 ,au moins 1 dans chaque paragraphe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Les liens en page accueil en haut de page++.</t>
+  </si>
+  <si>
+    <t>Vérifier que la compression ai bien été activée, les fichiers sont 'ils minifiés? Les caractères inutiles sont ils retirés?</t>
+  </si>
+  <si>
+    <t>Stockage données dans un cache , zone temporaire gagne tempspour le chargeent de la page.</t>
+  </si>
+  <si>
+    <t>Les mots clés doivent apparaitre,  les metas qui facilitent le SEO doivent apparaitrent soit title description content type robot canonical (contentu compréhensible)</t>
+  </si>
+  <si>
+    <t>Tout site doit être respondive avec version mobile ++</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif= ALLEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.reduction taille manuelle </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">découper limage + compression avec compressor  https://compressor.io/  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et changement du format</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://app.kwfinder.com/ </t>
+  </si>
+  <si>
+    <t>balise metas manquantes: title description canonical  robot + manque mot clés  .</t>
+  </si>
+  <si>
+    <t>Responsive pas adapté, google utilise la version mobile pour le classement et l'indexation .</t>
+  </si>
+  <si>
+    <t>Fichiers trop lourds , css et js 14% du poid total de la page web (source httparchive).</t>
+  </si>
+  <si>
+    <t>Le contenu est mal organisé: ordre des titres et leur mots clés, contenu vide li.</t>
+  </si>
+  <si>
+    <t>Les images sont trop lourdes et le format n'est pas adapté : .bmp .</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mauvais contraste texte dans image, </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color rgb="FF7030A0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t>bloc3 et bloc 1 et bloc footer,au niveau du logo la chouette A,du bouton contact.</t>
+    </r>
+  </si>
+  <si>
+    <t>Le texte est dans limage , la citation est consiérée comme une image ainsi qu'un titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La langue de la page mal définie    </t>
+  </si>
+  <si>
+    <r>
+      <t>Le formulaire de saisie page 2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">mauvais contraste texte dans image, </t>
-    </r>
-    <r>
-      <rPr>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FF7030A0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>bloc3 et bloc 1 et bloc footer,au niveau du logo la chouette A,du bouton contact</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">liens vident au niveaux des réseaux sociaux et liens redondants entre accueil et contact et contactez notre équipe </t>
-  </si>
-  <si>
-    <t>soit on en enlève les liens soit on apporte du texte pour décrire leur fonctionalité ,</t>
-  </si>
-  <si>
-    <t>equivalent textuel " alt" qui décrit succintement limage mais avec mot clé pour referencement  5 à 6 mots précis , il ne faut pas répéter le même alt</t>
-  </si>
-  <si>
-    <t>h1 puis h3 puis h2   , pas de mot clés dans les titres  et manque dans paragraphe</t>
-  </si>
-  <si>
-    <t>non perceptible , contraste visuel non suffisant pour les personnes à capacité visuelle réduite</t>
-  </si>
-  <si>
-    <t>trop lourdes , telechargement trop long: la taille est modifié via le css</t>
-  </si>
-  <si>
-    <t>les liens vers reseauux sociaux sont vident  ne sont pas compréhensibles pour l'utilisateur et n'apporte rien au site . Redondances sur la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WCA G2 w3c working group note AA , wave web evaluation tool, </t>
-  </si>
-  <si>
-    <t>WCA G2 w3c working group note AA , wave web evaluation tool, mdn web doc ,  https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-contrast.html</t>
-  </si>
-  <si>
-    <t>WCA G2 w3c working group note AA                                                                 https://www.w3.org/TR/UNDERSTANDING-WCAG20/consistent-behavior-consistent-locations.html</t>
-  </si>
-  <si>
-    <t>police des paragraphes trop petites ,la chouette agence police trop petite</t>
-  </si>
-  <si>
-    <r>
-      <t>WCA G2 w3c working group note</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> A                                                                   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-parses.html</t>
-    </r>
-  </si>
-  <si>
-    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941044-inspectez-manuellement-le-contenu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/TR/UNDERSTANDING-WCAG20/content-structure-separation-programmatic.html     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941044-inspectez-manuellement-le-contenu </t>
-  </si>
-  <si>
-    <r>
-      <t>WCA G2 w3c working group note</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> A                         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    https://www.balisemeta.com/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>WCA G2 w3c working group note</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> A     </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">                  wave web evaluation tool   , https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-parses.html      https://validator.w3.org/nu/?doc=https%3A%2F%2Flazouz44.github.io%2Fla-chouette-agence%2F</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=créer une design visuel accessible avec les contrastes de couleur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.augmenter le contraste entre le texte et background</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">test avec </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>contrast analizer  web-color.alias</t>
-    </r>
-  </si>
-  <si>
-    <t>le alt  ne décrit pas bien  chaque image(paris au lieu de lyon par ex)/ redondance au niveau de 2 alt avec même description</t>
-  </si>
-  <si>
-    <t>les erreures doivent etre clairement décrites, il doit y avoir des instructions , réécrire le code formulaire</t>
-  </si>
-  <si>
-    <t>pas d'indication  à l'entrée des informations , pas etiquette: pause pb pour le lecteur d'écran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">image doit avoir l même taille que son contenant </t>
-  </si>
-  <si>
-    <t>les mots clés doivent apparaitre,  les metas qui facilitent le SEO doivent apparaitrent soit title description content type robot canonical (contentu compréhensible)</t>
-  </si>
-  <si>
-    <t>le contenue ne sadapte mal au mobile : des images ne sont pas lisibles .</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=augmenter le trafic avec un site responsive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> .créer une super version mobile avec images titres bien visibles </t>
-    </r>
-  </si>
-  <si>
-    <t>liens partenaires en bas de page ++ balxk hat a supprimé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">du texte invisible est créé en haut à gauche pour stocker des mots clés cest du black hat trompe google ,  très mauvaise pratique </t>
-  </si>
-  <si>
-    <t>SEO on page  choisi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accessibilité </t>
-  </si>
-  <si>
-    <t>de faux liens sont utllisé au niveau de l'annuaire et partenariat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">il faut les enlever et au mieux rajouter de vrais liens externes et vrais partenariariat qui apportent quelque chose au site </t>
-  </si>
-  <si>
-    <t>objectif=être partagé sur les réseaux sociaux, augmenter l'autorité du site    , renseigner les liens , retirer les liens redondant (garder contact)</t>
-  </si>
-  <si>
-    <t>objectif=rendre le menu lisible il faut deplacer le menu pour quil soit visible</t>
-  </si>
-  <si>
-    <t>objectif= rendre le contenu utilisable et avec de bonnes pratiques</t>
-  </si>
-  <si>
-    <t>accessibilité choisi</t>
-  </si>
-  <si>
-    <t>objectif=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdn web doc  https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-text-presentation.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WCA G2 w3c working group note / Optimiz me  /   wave web evaluation tool  ,  https://www.w3.org/TR/UNDERSTANDING-WCAG20/text-equiv-all.html  working group note AA  </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">pratique black hat : de faux liens sont utilisés au niveau du footer </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  oke</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">le texte est dans limage , la citation  et le titre </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> oke</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">langue de la page mal définie    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>oke</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">creation de div keyords non  autorisées texte trop petit     black hat   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>oke</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">balise metas manquantes: title description canonical  robot + manque mot clés  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">oke </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>formulaire de saisie page 2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> zone de texte a rajouter</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>fichiers trop lourds , css et js 14% du poid total de la page web (source httparchive)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ala fin</t>
-    </r>
+      <t>n'est pas bien renseigné , le libellé n'est pas bien crée</t>
+    </r>
+  </si>
+  <si>
+    <t>Le contenue s4adapte au mobile mais il reste des modifications à apporter: des images ne sont pas lisibles .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il n'y a pas de travail sur mots clés ,  pas de présentation entreprise, </t>
+  </si>
+  <si>
+    <t>Contraste  visuel non suffisant pour les personnes à capacité visuelle réduite, le texte est non perceptible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De faux liens sont utllisés au niveau de l'annuaire et partenariats, du texte invisible est créé en haut à gauche pour stocker des mots clés  , </t>
+  </si>
+  <si>
+    <t>Les liens vers reseauux sociaux sont vident ? ne sont pas compréhensibles pour l'utilisateur et n'apporte rien au site . Redondances sur la page</t>
+  </si>
+  <si>
+    <t>Soit on en enlève les liens soit on apporte du texte pour décrire leur fonctionalité ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il faut les enlever et au mieux rajouter de vrais liens externes et vrais partenariariat qui apportent quelque chose au site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il faut que le contenu soit liible perceptible comprehensible </t>
+  </si>
+  <si>
+    <t>Les erreures doivent etre clairement décrites, il doit y avoir des instructions , réécrire le code formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Définir correctement la langue de la page </t>
+  </si>
+  <si>
+    <t>Equivalent textuel " alt" qui décrit succintement limage mais avec mot clé pour referencement  5 à 6 mots précis , il ne faut pas répéter le même alt</t>
+  </si>
+  <si>
+    <t>Le texte doit etre en dehors de limage , les images avec du texte doivent être évités</t>
+  </si>
+  <si>
+    <t>Le contenu doit etre bien segmenté,contenu optimisé avec des elements html structurels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">règles WCAG contraste doit etre de 3,1(pour texte de grande taille).  le contraste entre le texte et larr plan de 4,5:1 pour texte normaux
+règles WCAG contreforme ouverte trait uniforme interlettrage et interligne </t>
+  </si>
+  <si>
+    <t>Il faut utliser hidden , visibility mais jamais utiliser lopacité nulle l'ordre des z index pour le masquage de contenu .l'élément doit être réelement invisible.</t>
+  </si>
+  <si>
+    <t>Mot clé web design dans url, c longue traine à privilégier , créer un google my business avec localisation, analyse google analitics</t>
   </si>
 </sst>
 </file>
@@ -1237,16 +1198,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="113" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="138" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="129.109375" customWidth="1"/>
+    <col min="3" max="3" width="126.77734375" customWidth="1"/>
+    <col min="4" max="4" width="146.44140625" customWidth="1"/>
     <col min="5" max="5" width="139" customWidth="1"/>
     <col min="6" max="6" width="212.77734375" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
@@ -1301,395 +1262,388 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
+      <c r="A3" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
+        <v>74</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
+        <v>72</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
+      <c r="A6" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
+        <v>56</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
+        <v>87</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>35</v>
+      <c r="A9" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
+      <c r="A10" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
+        <v>86</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
+      <c r="F11" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
+      <c r="A13" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>100</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>97</v>
-      </c>
+      <c r="A23" s="6"/>
       <c r="B23" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>96</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2678,8 +2632,9 @@
     <hyperlink ref="F3" r:id="rId4"/>
     <hyperlink ref="F10" r:id="rId5"/>
     <hyperlink ref="F21" r:id="rId6"/>
+    <hyperlink ref="F11" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId7"/>
+  <pageSetup orientation="landscape" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modif responsive image centrée au zoom et sur page d'accueil, css enlevé pour le nav , reste l'adresse page 2 sur le côté.
</commit_message>
<xml_diff>
--- a/cour/Modèle-audit-SEO (1).xlsx
+++ b/cour/Modèle-audit-SEO (1).xlsx
@@ -42,9 +42,6 @@
     <t>(SEO ou accessiblité ?)</t>
   </si>
   <si>
-    <t>téléchargement non optimisé</t>
-  </si>
-  <si>
     <t>site pas mis en valeur</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>décalé sur la droite nest pas lisible /accessible/ pas cohérent par rapport a page d'accueil/ toggle nav nexiste pas sur la page d'accueil</t>
   </si>
   <si>
-    <t xml:space="preserve">incohérance dans l'interface, le contenu nest pas compréhensible page 2 on ne voit pas le menu et toggle nav </t>
-  </si>
-  <si>
     <t>on page/ SEO  choisi</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>pas une bonne lisibilité , la typo n'est pas accesible car aperture fermée</t>
   </si>
   <si>
-    <t>les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -150,12 +141,6 @@
   </si>
   <si>
     <t xml:space="preserve">SEO on page </t>
-  </si>
-  <si>
-    <t>pas de cache navigateur:zone de stockage temporaire et rapide ( pas installable avec git hub)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liens vident au niveaux des réseaux sociaux et liens redondants entre accueil et contact et contactez notre équipe </t>
   </si>
   <si>
     <t xml:space="preserve">WCA G2 w3c working group note AA , wave web evaluation tool, </t>
@@ -292,9 +277,6 @@
     <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site</t>
   </si>
   <si>
-    <t xml:space="preserve">liens partenaires en bas de page </t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -731,47 +713,33 @@
     <t>Les images sont trop lourdes et le format n'est pas adapté : .bmp .</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">mauvais contraste texte dans image, </t>
-    </r>
-    <r>
-      <rPr>
+    <t>Le texte est dans limage , la citation est consiérée comme une image ainsi qu'un titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La langue de la page mal définie    </t>
+  </si>
+  <si>
+    <r>
+      <t>Le formulaire de saisie page 2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FF7030A0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>bloc3 et bloc 1 et bloc footer,au niveau du logo la chouette A,du bouton contact.</t>
-    </r>
-  </si>
-  <si>
-    <t>Le texte est dans limage , la citation est consiérée comme une image ainsi qu'un titre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La langue de la page mal définie    </t>
-  </si>
-  <si>
-    <r>
-      <t>Le formulaire de saisie page 2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>n'est pas bien renseigné , le libellé n'est pas bien crée</t>
     </r>
   </si>
@@ -847,13 +815,34 @@
   </si>
   <si>
     <t>accessibilité     optimisation technique     choisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liens partenaires en bas de page </t>
+  </si>
+  <si>
+    <t>Les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incohérance dans l'interface, le contenu nest pas compréhensible page 2 on ne voit pas le menu et toggle nav </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liens vident au niveaux des réseaux sociaux et liens redondants entre accueil et contact et contactez notre équipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cache navigateur mal paramétré : c'est unezone de stockage temporaire et rapide . Ca durée de vie est ici de 10 minutes ( pas installable avec git hub)</t>
+  </si>
+  <si>
+    <t>téléchargement non optimisé, la durée de vie du cache devrait être d'au moins 1 heure .</t>
+  </si>
+  <si>
+    <t>mauvais contraste texte dans image,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -914,12 +903,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF7030A0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -971,7 +954,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -988,7 +971,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1205,7 +1188,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1269,42 +1252,42 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1312,342 +1295,342 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="F11" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="C13" s="6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C23" s="6"/>
     </row>

</xml_diff>

<commit_message>
amélioration html , correction accolade en trop css minifié
</commit_message>
<xml_diff>
--- a/cour/Modèle-audit-SEO (1).xlsx
+++ b/cour/Modèle-audit-SEO (1).xlsx
@@ -553,7 +553,143 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">pratique black hat : de faux liens sont utilisés au niveau du footer </t>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> rendre le contenu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>UTILISABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et avec de bonnes pratiques</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SEO on page       choisi</t>
+  </si>
+  <si>
+    <t>h1 puis h3 puis h2   , pas de mots clés dans les titres  et manque dans paragraphe.</t>
+  </si>
+  <si>
+    <t>Les liens permettent d'augmenter l'autorité et donc l'accessibilité, doivent être de qualité et au mieux en  haut de page.</t>
+  </si>
+  <si>
+    <t>Trop lourdes , téléchargement trop long: la taille est modifiée via le css , le format nest pas optimum .</t>
+  </si>
+  <si>
+    <t>Ne facilitent pas le téléchargement car les fichiers sont  trop lourds : css js , html</t>
+  </si>
+  <si>
+    <t>L'image doit avoir la même taille que son contenant ou plus petite.Il faut privilégier les formats jpg, png voir jpeg 2000 .</t>
+  </si>
+  <si>
+    <t>Le contenu doit être utilisable: h1 h2 bien structuré du plus spécifique au plus général, avec des mot clés , mots clés ou synonyme pour h2 ,au moins 1 dans chaque paragraphe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Les liens en page accueil en haut de page++.</t>
+  </si>
+  <si>
+    <t>Vérifier que la compression ai bien été activée, les fichiers sont 'ils minifiés? Les caractères inutiles sont ils retirés?</t>
+  </si>
+  <si>
+    <t>Stockage données dans un cache , zone temporaire gagne tempspour le chargeent de la page.</t>
+  </si>
+  <si>
+    <t>Les mots clés doivent apparaitre,  les metas qui facilitent le SEO doivent apparaitrent soit title description content type robot canonical (contentu compréhensible)</t>
+  </si>
+  <si>
+    <t>Tout site doit être respondive avec version mobile ++</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>objectif= ALLEGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.reduction taille manuelle </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">découper limage + compression avec compressor  https://compressor.io/  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> et changement du format</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://app.kwfinder.com/ </t>
+  </si>
+  <si>
+    <t>balise metas manquantes: title description canonical  robot + manque mot clés  .</t>
+  </si>
+  <si>
+    <t>Responsive pas adapté, google utilise la version mobile pour le classement et l'indexation .</t>
+  </si>
+  <si>
+    <t>Fichiers trop lourds , css et js 14% du poid total de la page web (source httparchive).</t>
+  </si>
+  <si>
+    <t>Les images sont trop lourdes et le format n'est pas adapté : .bmp .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La langue de la page mal définie    </t>
+  </si>
+  <si>
+    <r>
+      <t>Le formulaire de saisie page 2</t>
     </r>
     <r>
       <rPr>
@@ -573,154 +709,112 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">et creation de div keyords non  autorisées texte trop petit      </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> rendre le contenu </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>UTILISABLE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et avec de bonnes pratiques</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>SEO on page       choisi</t>
-  </si>
-  <si>
-    <t>h1 puis h3 puis h2   , pas de mots clés dans les titres  et manque dans paragraphe.</t>
-  </si>
-  <si>
-    <t>Les liens permettent d'augmenter l'autorité et donc l'accessibilité, doivent être de qualité et au mieux en  haut de page.</t>
-  </si>
-  <si>
-    <t>Trop lourdes , téléchargement trop long: la taille est modifiée via le css , le format nest pas optimum .</t>
-  </si>
-  <si>
-    <t>Ne facilitent pas le téléchargement car les fichiers sont  trop lourds : css js , html</t>
-  </si>
-  <si>
-    <t>L'image doit avoir la même taille que son contenant ou plus petite.Il faut privilégier les formats jpg, png voir jpeg 2000 .</t>
-  </si>
-  <si>
-    <t>Le contenu doit être utilisable: h1 h2 bien structuré du plus spécifique au plus général, avec des mot clés , mots clés ou synonyme pour h2 ,au moins 1 dans chaque paragraphe.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Les liens en page accueil en haut de page++.</t>
-  </si>
-  <si>
-    <t>Vérifier que la compression ai bien été activée, les fichiers sont 'ils minifiés? Les caractères inutiles sont ils retirés?</t>
-  </si>
-  <si>
-    <t>Stockage données dans un cache , zone temporaire gagne tempspour le chargeent de la page.</t>
-  </si>
-  <si>
-    <t>Les mots clés doivent apparaitre,  les metas qui facilitent le SEO doivent apparaitrent soit title description content type robot canonical (contentu compréhensible)</t>
-  </si>
-  <si>
-    <t>Tout site doit être respondive avec version mobile ++</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectif= ALLEGER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.reduction taille manuelle </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">découper limage + compression avec compressor  https://compressor.io/  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> et changement du format</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">https://app.kwfinder.com/ </t>
-  </si>
-  <si>
-    <t>balise metas manquantes: title description canonical  robot + manque mot clés  .</t>
-  </si>
-  <si>
-    <t>Responsive pas adapté, google utilise la version mobile pour le classement et l'indexation .</t>
-  </si>
-  <si>
-    <t>Fichiers trop lourds , css et js 14% du poid total de la page web (source httparchive).</t>
-  </si>
-  <si>
-    <t>Le contenu est mal organisé: ordre des titres et leur mots clés, contenu vide li.</t>
-  </si>
-  <si>
-    <t>Les images sont trop lourdes et le format n'est pas adapté : .bmp .</t>
-  </si>
-  <si>
-    <t>Le texte est dans limage , la citation est consiérée comme une image ainsi qu'un titre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La langue de la page mal définie    </t>
-  </si>
-  <si>
-    <r>
-      <t>Le formulaire de saisie page 2</t>
+      <t>n'est pas bien renseigné , le libellé n'est pas bien crée</t>
+    </r>
+  </si>
+  <si>
+    <t>Le contenue s4adapte au mobile mais il reste des modifications à apporter: des images ne sont pas lisibles .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il n'y a pas de travail sur mots clés ,  pas de présentation entreprise, </t>
+  </si>
+  <si>
+    <t>Contraste  visuel non suffisant pour les personnes à capacité visuelle réduite, le texte est non perceptible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De faux liens sont utllisés au niveau de l'annuaire et partenariats, du texte invisible est créé en haut à gauche pour stocker des mots clés  , </t>
+  </si>
+  <si>
+    <t>Les liens vers reseauux sociaux sont vident ? ne sont pas compréhensibles pour l'utilisateur et n'apporte rien au site . Redondances sur la page</t>
+  </si>
+  <si>
+    <t>Soit on en enlève les liens soit on apporte du texte pour décrire leur fonctionalité ,</t>
+  </si>
+  <si>
+    <t>Il faut utliser hidden , visibility mais jamais utiliser lopacité nulle l'ordre des z index pour le masquage de contenu .l'élément doit être réelement invisible.</t>
+  </si>
+  <si>
+    <t>Définir correctement la langue de la page .</t>
+  </si>
+  <si>
+    <t>Il faut que le contenu soit liible perceptible comprehensible .</t>
+  </si>
+  <si>
+    <t>Il faut les enlever et au mieux rajouter de vrais liens externes et vrais partenariariats qui apportent quelque chose au site .</t>
+  </si>
+  <si>
+    <t>Equivalent textuel " alt" qui décrit succintement l'image mais avec des mots clés pour le référencement  5 à 6 mots précis , il ne faut pas répéter le même alt.</t>
+  </si>
+  <si>
+    <t>Le texte doit etre en dehors de limage , les images avec du texte doivent être évités.</t>
+  </si>
+  <si>
+    <t>Le contenu doit être bien segmenté,contenu optimisé avec des éléments html structurels.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">règles WCAG contraste doit être de 3,1(pour texte de grande taille).  le contraste entre le texte et larr plan de 4,5:1 pour texte normaux .
+règles WCAG contreforme ouverte trait uniforme interlettrage et interligne </t>
+  </si>
+  <si>
+    <t>regles WCAG aperture ouverte trait uniforme .</t>
+  </si>
+  <si>
+    <t>Mot clé web design dans url, chaîne longue traine à privilégier , créer un google my business avec localisation, analyse google analitics.</t>
+  </si>
+  <si>
+    <t>Les erreures doivent être clairement décrites,  , réécrire le code formulaire.</t>
+  </si>
+  <si>
+    <t>vitesse/taille SEO on page  choisi</t>
+  </si>
+  <si>
+    <t>vitesse/taille SEO optimisation texhnique  choisi</t>
+  </si>
+  <si>
+    <t>vitesse SEO on page         choisi</t>
+  </si>
+  <si>
+    <t>SEO   optimisation technique     choisi</t>
+  </si>
+  <si>
+    <t>accessibilité    optimisaton technique      choisi</t>
+  </si>
+  <si>
+    <t>accessibilité     optimisation technique   choisi</t>
+  </si>
+  <si>
+    <t>accessibilité     optimisation technique     choisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liens partenaires en bas de page </t>
+  </si>
+  <si>
+    <t>Les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incohérance dans l'interface, le contenu nest pas compréhensible page 2 on ne voit pas le menu et toggle nav </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liens vident au niveaux des réseaux sociaux et liens redondants entre accueil et contact et contactez notre équipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cache navigateur mal paramétré : c'est unezone de stockage temporaire et rapide . Ca durée de vie est ici de 10 minutes ( pas installable avec git hub)</t>
+  </si>
+  <si>
+    <t>téléchargement non optimisé, la durée de vie du cache devrait être d'au moins 1 heure .</t>
+  </si>
+  <si>
+    <t>mauvais contraste texte dans image,</t>
+  </si>
+  <si>
+    <t>Le texte est dans limage , la citation est considérée comme une image ainsi qu'un titre</t>
+  </si>
+  <si>
+    <t>Le contenu est mal organisé: ordre des titres et leur mots clés, contenu vide li, balises structurantes manquantes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pratique black hat : de faux liens sont utilisés au niveau du footer </t>
     </r>
     <r>
       <rPr>
@@ -740,109 +834,15 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>n'est pas bien renseigné , le libellé n'est pas bien crée</t>
-    </r>
-  </si>
-  <si>
-    <t>Le contenue s4adapte au mobile mais il reste des modifications à apporter: des images ne sont pas lisibles .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il n'y a pas de travail sur mots clés ,  pas de présentation entreprise, </t>
-  </si>
-  <si>
-    <t>Contraste  visuel non suffisant pour les personnes à capacité visuelle réduite, le texte est non perceptible.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De faux liens sont utllisés au niveau de l'annuaire et partenariats, du texte invisible est créé en haut à gauche pour stocker des mots clés  , </t>
-  </si>
-  <si>
-    <t>Les liens vers reseauux sociaux sont vident ? ne sont pas compréhensibles pour l'utilisateur et n'apporte rien au site . Redondances sur la page</t>
-  </si>
-  <si>
-    <t>Soit on en enlève les liens soit on apporte du texte pour décrire leur fonctionalité ,</t>
-  </si>
-  <si>
-    <t>Il faut utliser hidden , visibility mais jamais utiliser lopacité nulle l'ordre des z index pour le masquage de contenu .l'élément doit être réelement invisible.</t>
-  </si>
-  <si>
-    <t>Définir correctement la langue de la page .</t>
-  </si>
-  <si>
-    <t>Il faut que le contenu soit liible perceptible comprehensible .</t>
-  </si>
-  <si>
-    <t>Il faut les enlever et au mieux rajouter de vrais liens externes et vrais partenariariats qui apportent quelque chose au site .</t>
-  </si>
-  <si>
-    <t>Equivalent textuel " alt" qui décrit succintement l'image mais avec des mots clés pour le référencement  5 à 6 mots précis , il ne faut pas répéter le même alt.</t>
-  </si>
-  <si>
-    <t>Le texte doit etre en dehors de limage , les images avec du texte doivent être évités.</t>
-  </si>
-  <si>
-    <t>Le contenu doit être bien segmenté,contenu optimisé avec des éléments html structurels.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">règles WCAG contraste doit être de 3,1(pour texte de grande taille).  le contraste entre le texte et larr plan de 4,5:1 pour texte normaux .
-règles WCAG contreforme ouverte trait uniforme interlettrage et interligne </t>
-  </si>
-  <si>
-    <t>regles WCAG aperture ouverte trait uniforme .</t>
-  </si>
-  <si>
-    <t>Mot clé web design dans url, chaîne longue traine à privilégier , créer un google my business avec localisation, analyse google analitics.</t>
-  </si>
-  <si>
-    <t>Les erreures doivent être clairement décrites,  , réécrire le code formulaire.</t>
-  </si>
-  <si>
-    <t>vitesse/taille SEO on page  choisi</t>
-  </si>
-  <si>
-    <t>vitesse/taille SEO optimisation texhnique  choisi</t>
-  </si>
-  <si>
-    <t>vitesse SEO on page         choisi</t>
-  </si>
-  <si>
-    <t>SEO   optimisation technique     choisi</t>
-  </si>
-  <si>
-    <t>accessibilité    optimisaton technique      choisi</t>
-  </si>
-  <si>
-    <t>accessibilité     optimisation technique   choisi</t>
-  </si>
-  <si>
-    <t>accessibilité     optimisation technique     choisi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liens partenaires en bas de page </t>
-  </si>
-  <si>
-    <t>Les images ne sont pas bien décrite avec alt , permet un meilleur positionnement via mots clés et génére du trafic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incohérance dans l'interface, le contenu nest pas compréhensible page 2 on ne voit pas le menu et toggle nav </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liens vident au niveaux des réseaux sociaux et liens redondants entre accueil et contact et contactez notre équipe </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cache navigateur mal paramétré : c'est unezone de stockage temporaire et rapide . Ca durée de vie est ici de 10 minutes ( pas installable avec git hub)</t>
-  </si>
-  <si>
-    <t>téléchargement non optimisé, la durée de vie du cache devrait être d'au moins 1 heure .</t>
-  </si>
-  <si>
-    <t>mauvais contraste texte dans image,</t>
+      <t xml:space="preserve">et creation de div keyords non  autorisées, texte trop petit      </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -921,6 +921,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -956,7 +962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -972,6 +978,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1187,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1251,37 +1258,37 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>98</v>
+      <c r="A3" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>48</v>
@@ -1298,30 +1305,30 @@
         <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>99</v>
+      <c r="A7" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>49</v>
@@ -1335,13 +1342,13 @@
         <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>50</v>
@@ -1351,17 +1358,17 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>100</v>
+      <c r="A9" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>23</v>
@@ -1371,17 +1378,17 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>101</v>
+      <c r="A10" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>40</v>
@@ -1398,16 +1405,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,24 +1428,24 @@
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>104</v>
+      <c r="A13" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>51</v>
@@ -1458,7 +1465,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>52</v>
@@ -1478,7 +1485,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>24</v>
@@ -1488,17 +1495,17 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>102</v>
+      <c r="A16" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>44</v>
@@ -1512,13 +1519,13 @@
         <v>28</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>53</v>
@@ -1528,17 +1535,17 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>103</v>
+      <c r="A18" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>54</v>
@@ -1548,17 +1555,17 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>103</v>
+      <c r="A19" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>55</v>
@@ -1572,13 +1579,13 @@
         <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>43</v>
@@ -1588,20 +1595,20 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>59</v>
+      <c r="A21" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>34</v>
@@ -1612,13 +1619,13 @@
         <v>28</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>42</v>
@@ -1630,7 +1637,7 @@
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="6"/>
     </row>

</xml_diff>